<commit_message>
Cập nhật báo cáo theo bẽnh nhân
</commit_message>
<xml_diff>
--- a/public/excel/baocao1.xlsx
+++ b/public/excel/baocao1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
   <si>
     <t>Thống Kê Bán Hàng Theo Bệnh Nhân</t>
   </si>
@@ -26,7 +26,7 @@
     <t>BỆNH VIỆN NHÂN ÁI</t>
   </si>
   <si>
-    <t>Từ ngày: 01-11-2021 đến ngày: 03-11-2022</t>
+    <t>Từ ngày: 01-11-2022 đến ngày: 01-11-2022</t>
   </si>
   <si>
     <t>STT</t>
@@ -59,127 +59,289 @@
     <t>Ghi Chú</t>
   </si>
   <si>
-    <t>Di Lee</t>
-  </si>
-  <si>
-    <t>Bạc hà</t>
+    <t>Lê Thiện Tâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Điện thoại </t>
+  </si>
+  <si>
+    <t>TSDTK</t>
+  </si>
+  <si>
+    <t>Phút</t>
+  </si>
+  <si>
+    <t>500,000đ</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Trần Thanh Toàn</t>
+  </si>
+  <si>
+    <t>Cơm tấm</t>
   </si>
   <si>
     <t>TPCB</t>
   </si>
   <si>
+    <t>hộp</t>
+  </si>
+  <si>
+    <t>30,000đ</t>
+  </si>
+  <si>
+    <t>Chuối</t>
+  </si>
+  <si>
     <t>kg</t>
   </si>
   <si>
-    <t>19,000đ</t>
-  </si>
-  <si>
-    <t>KN001</t>
-  </si>
-  <si>
-    <t>38,000đ</t>
-  </si>
-  <si>
-    <t>Cad điện thoại</t>
-  </si>
-  <si>
-    <t>TSDTK</t>
-  </si>
-  <si>
-    <t>cái</t>
-  </si>
-  <si>
-    <t>80,000đ</t>
+    <t>13,000đ</t>
+  </si>
+  <si>
+    <t>Trần Thị Kim Dung</t>
+  </si>
+  <si>
+    <t>Băng vệ sinh Diana</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Gói</t>
+  </si>
+  <si>
+    <t>24,000đ</t>
+  </si>
+  <si>
+    <t>Bánh canh</t>
+  </si>
+  <si>
+    <t>tô</t>
+  </si>
+  <si>
+    <t>Trần Phát Tuyến</t>
+  </si>
+  <si>
+    <t>Trà bảo tín</t>
+  </si>
+  <si>
+    <t>11,000đ</t>
+  </si>
+  <si>
+    <t>22,000đ</t>
+  </si>
+  <si>
+    <t>Kẹo cà phê</t>
+  </si>
+  <si>
+    <t>18,000đ</t>
+  </si>
+  <si>
+    <t>Nguyễn Hiếu Cường</t>
+  </si>
+  <si>
+    <t>33,000đ</t>
+  </si>
+  <si>
+    <t>Trịnh Thị Quỳnh</t>
+  </si>
+  <si>
+    <t>Nước bò húc</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>14,000đ</t>
+  </si>
+  <si>
+    <t>28,000đ</t>
+  </si>
+  <si>
+    <t>Nước number one</t>
+  </si>
+  <si>
+    <t>10,000đ</t>
+  </si>
+  <si>
+    <t>Nguyễn Thái Hân</t>
+  </si>
+  <si>
+    <t>26,000đ</t>
+  </si>
+  <si>
+    <t>Trứng gà</t>
+  </si>
+  <si>
+    <t>quả</t>
+  </si>
+  <si>
+    <t>3,000đ</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Hào</t>
+  </si>
+  <si>
+    <t>Cà phê việt</t>
+  </si>
+  <si>
+    <t>Hộp</t>
+  </si>
+  <si>
+    <t>66,000đ</t>
+  </si>
+  <si>
+    <t>Dầu gội Clear trung</t>
+  </si>
+  <si>
+    <t>110,000đ</t>
+  </si>
+  <si>
+    <t>Xà bông ô mô</t>
+  </si>
+  <si>
+    <t>42,000đ</t>
+  </si>
+  <si>
+    <t>Cà phê phố</t>
+  </si>
+  <si>
+    <t>46,000đ</t>
+  </si>
+  <si>
+    <t>PHAN THÀNH CÔNG</t>
+  </si>
+  <si>
+    <t>Chao bông mai</t>
+  </si>
+  <si>
+    <t>Hủ</t>
+  </si>
+  <si>
+    <t>15,000đ</t>
+  </si>
+  <si>
+    <t>Trần Kim Phụng</t>
+  </si>
+  <si>
+    <t>Dầu xả comfor + dwny</t>
+  </si>
+  <si>
+    <t>2,500đ</t>
+  </si>
+  <si>
+    <t>Hồ Hữu Quới</t>
+  </si>
+  <si>
+    <t>56,000đ</t>
   </si>
   <si>
     <t>40,000đ</t>
   </si>
   <si>
-    <t>Bánh cam</t>
-  </si>
-  <si>
-    <t>3,500đ</t>
-  </si>
-  <si>
-    <t>Lâm Tú Ngân</t>
-  </si>
-  <si>
-    <t>Bánh bông lan</t>
-  </si>
-  <si>
-    <t>11,000đ</t>
-  </si>
-  <si>
-    <t>Huylq</t>
-  </si>
-  <si>
-    <t>Bánh bèo</t>
-  </si>
-  <si>
-    <t>hộp</t>
+    <t>Mai Minh Đăng</t>
+  </si>
+  <si>
+    <t>Bắp cải</t>
+  </si>
+  <si>
+    <t>31,000đ</t>
+  </si>
+  <si>
+    <t>Cà chua</t>
+  </si>
+  <si>
+    <t>0,5kg</t>
   </si>
   <si>
     <t>17,000đ</t>
   </si>
   <si>
-    <t>KN002</t>
-  </si>
-  <si>
-    <t>Bánh cưốn chả</t>
-  </si>
-  <si>
-    <t>Bánh chưng nhỏ</t>
-  </si>
-  <si>
-    <t>cây</t>
-  </si>
-  <si>
-    <t>Lê Thanh Vinh</t>
-  </si>
-  <si>
-    <t>10,000đ</t>
-  </si>
-  <si>
-    <t>Tất Tiến Vinh</t>
-  </si>
-  <si>
-    <t>Bột lộc</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Vũ</t>
-  </si>
-  <si>
-    <t>Bắp cải</t>
-  </si>
-  <si>
-    <t>0,5kg</t>
+    <t>Cải chua</t>
+  </si>
+  <si>
+    <t>Ruốc</t>
+  </si>
+  <si>
+    <t>0,1kg</t>
+  </si>
+  <si>
+    <t>45,000đ</t>
+  </si>
+  <si>
+    <t>Bột ngọt</t>
+  </si>
+  <si>
+    <t>9,000đ</t>
+  </si>
+  <si>
+    <t>Bột nêm</t>
+  </si>
+  <si>
+    <t>20,000đ</t>
+  </si>
+  <si>
+    <t>Đường cát</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Kẹo đậu hội giang</t>
+  </si>
+  <si>
+    <t>44,000đ</t>
+  </si>
+  <si>
+    <t>Tương ớt</t>
+  </si>
+  <si>
+    <t>Chai</t>
+  </si>
+  <si>
+    <t>Ngô Trường Tâm</t>
+  </si>
+  <si>
+    <t>84,000đ</t>
+  </si>
+  <si>
+    <t>132,000đ</t>
+  </si>
+  <si>
+    <t>300,000đ</t>
+  </si>
+  <si>
+    <t>Nguyễn Ý Thức</t>
+  </si>
+  <si>
+    <t>Ớt trái</t>
+  </si>
+  <si>
+    <t>8,000đ</t>
   </si>
   <si>
     <t>16,000đ</t>
   </si>
   <si>
-    <t>Bánh ướt</t>
-  </si>
-  <si>
-    <t>Bánh cuốn</t>
-  </si>
-  <si>
-    <t>Cà chua</t>
-  </si>
-  <si>
-    <t>Cà pháo</t>
-  </si>
-  <si>
-    <t>14,000đ</t>
-  </si>
-  <si>
-    <t>Cải thìa</t>
-  </si>
-  <si>
-    <t>Bột năng</t>
-  </si>
-  <si>
-    <t>0,1kg</t>
+    <t>Hủ tiếu</t>
+  </si>
+  <si>
+    <t>60,000đ</t>
+  </si>
+  <si>
+    <t>Mì hảo hảo</t>
+  </si>
+  <si>
+    <t>5,000đ</t>
+  </si>
+  <si>
+    <t>50,000đ</t>
+  </si>
+  <si>
+    <t>100,000đ</t>
   </si>
   <si>
     <t>Người lập</t>
@@ -571,19 +733,19 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J48" sqref="J48"/>
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="6" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="10" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -680,10 +842,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -692,7 +854,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>21</v>
@@ -722,19 +884,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>19</v>
@@ -743,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -752,19 +914,19 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
@@ -773,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -782,19 +944,19 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>19</v>
@@ -803,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -812,28 +974,28 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -842,19 +1004,19 @@
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>19</v>
@@ -863,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -872,28 +1034,28 @@
         <v>8</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H13" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -902,28 +1064,28 @@
         <v>9</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="H14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -932,28 +1094,26 @@
         <v>10</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="H15" s="5">
         <v>1</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="J15" s="5"/>
     </row>
@@ -962,28 +1122,28 @@
         <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="H16" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -992,28 +1152,28 @@
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="5">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H17" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="J17" s="5"/>
     </row>
@@ -1022,28 +1182,28 @@
         <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="5">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H18" s="5">
         <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="J18" s="5"/>
     </row>
@@ -1052,28 +1212,26 @@
         <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H19" s="5">
         <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J19" s="5"/>
     </row>
@@ -1082,28 +1240,26 @@
         <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="5">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="J20" s="5"/>
     </row>
@@ -1112,28 +1268,28 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="5">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H21" s="5">
         <v>1</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="J21" s="5"/>
     </row>
@@ -1142,28 +1298,28 @@
         <v>17</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="5">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H22" s="5">
         <v>1</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="J22" s="5"/>
     </row>
@@ -1172,28 +1328,28 @@
         <v>18</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H23" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1202,28 +1358,28 @@
         <v>19</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="5">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H24" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1232,28 +1388,26 @@
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="5">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H25" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="J25" s="5"/>
     </row>
@@ -1262,28 +1416,28 @@
         <v>21</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" s="5">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H26" s="5">
         <v>1</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="J26" s="5"/>
     </row>
@@ -1292,28 +1446,28 @@
         <v>22</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="5">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H27" s="5">
         <v>1</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="J27" s="5"/>
     </row>
@@ -1322,28 +1476,28 @@
         <v>23</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28" s="5">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H28" s="5">
         <v>1</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="J28" s="5"/>
     </row>
@@ -1352,28 +1506,28 @@
         <v>24</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H29" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="J29" s="5"/>
     </row>
@@ -1382,28 +1536,28 @@
         <v>25</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H30" s="5">
         <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="J30" s="5"/>
     </row>
@@ -1412,28 +1566,26 @@
         <v>26</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H31" s="5">
         <v>1</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="J31" s="5"/>
     </row>
@@ -1442,28 +1594,28 @@
         <v>27</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="5">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H32" s="5">
         <v>1</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="J32" s="5"/>
     </row>
@@ -1472,28 +1624,28 @@
         <v>28</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="5">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="J33" s="5"/>
     </row>
@@ -1502,28 +1654,28 @@
         <v>29</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" s="5">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H34" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="J34" s="5"/>
     </row>
@@ -1532,28 +1684,28 @@
         <v>30</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H35" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="J35" s="5"/>
     </row>
@@ -1562,28 +1714,28 @@
         <v>31</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" s="5">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H36" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="J36" s="5"/>
     </row>
@@ -1592,28 +1744,28 @@
         <v>32</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="5">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H37" s="5">
         <v>1</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="J37" s="5"/>
     </row>
@@ -1622,28 +1774,28 @@
         <v>33</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G38" s="5">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H38" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="J38" s="5"/>
     </row>
@@ -1652,28 +1804,26 @@
         <v>34</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G39" s="5">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H39" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="J39" s="5"/>
     </row>
@@ -1682,28 +1832,28 @@
         <v>35</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G40" s="5">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H40" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="J40" s="5"/>
     </row>
@@ -1712,28 +1862,28 @@
         <v>36</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G41" s="5">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H41" s="5">
         <v>1</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="J41" s="5"/>
     </row>
@@ -1742,246 +1892,66 @@
         <v>37</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G42" s="5">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H42" s="5">
         <v>1</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="5">
-        <v>38</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H43" s="5">
-        <v>1</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J43" s="5"/>
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="5">
-        <v>39</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H44" s="5">
-        <v>1</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="5">
-        <v>40</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H45" s="5">
-        <v>1</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="5">
-        <v>41</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H46" s="5">
-        <v>1</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="5">
-        <v>42</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" s="5">
-        <v>1</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J47" s="5"/>
+      <c r="A44"/>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44"/>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44" t="s">
+        <v>111</v>
+      </c>
+      <c r="H44"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="5">
-        <v>43</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H48" s="5">
-        <v>1</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="H49"/>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50"/>
-      <c r="B50" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50"/>
-      <c r="D50" t="s">
-        <v>56</v>
-      </c>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50" t="s">
-        <v>57</v>
-      </c>
-      <c r="H50"/>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54"/>
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>